<commit_message>
updated from desktop folder
</commit_message>
<xml_diff>
--- a/data/keion/ISU Fall 2022 Soil test results wlp modified.xlsx
+++ b/data/keion/ISU Fall 2022 Soil test results wlp modified.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/My Drive/r_class_2024_fall/data/keion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Desktop/R_class_2024/data/keion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DF3D49-0FE2-AC44-AE3D-A56C98901C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEA9FBC-07CE-E74E-9F87-8A0E43DCB181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44160" yWindow="2660" windowWidth="28280" windowHeight="19680" activeTab="1" xr2:uid="{3901E9A2-4BDE-41B5-8BF0-2CC1C0037FC4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="31">
   <si>
     <t>ISU</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>WIU</t>
-  </si>
-  <si>
-    <t>)</t>
   </si>
   <si>
     <t>index</t>
@@ -535,34 +532,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -7487,8 +7484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8EC270-F2FC-42BE-88F5-F89DEA2D7A05}">
   <dimension ref="A1:J217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I200" sqref="I200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7500,34 +7497,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -13890,9 +13887,6 @@
       </c>
       <c r="H200">
         <v>65.2</v>
-      </c>
-      <c r="I200" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="J200">
         <v>281</v>

</xml_diff>